<commit_message>
freq option add timestamp combine
</commit_message>
<xml_diff>
--- a/AD_Log.xlsx
+++ b/AD_Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yagciilk\Documents\Arduino\Pangolin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31031dea7aa373a1/Belgeler/Arduino/Proximab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D736962-7687-49C5-9C99-127A3C14751E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{0D736962-7687-49C5-9C99-127A3C14751E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EE3A8DE-2AEB-4AC3-ABF5-46D5A19CEC2F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -590,7 +590,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -935,16 +935,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -994,7 +994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
uC uniqe Id added
</commit_message>
<xml_diff>
--- a/AD_Log.xlsx
+++ b/AD_Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31031dea7aa373a1/Belgeler/Arduino/Proximab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{0D736962-7687-49C5-9C99-127A3C14751E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EE3A8DE-2AEB-4AC3-ABF5-46D5A19CEC2F}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{0D736962-7687-49C5-9C99-127A3C14751E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4598ECFD-D585-47B6-9EAC-A67C87B8C863}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -939,10 +939,14 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
+    <col min="9" max="9" width="34.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>